<commit_message>
feat: add test: check that the text is blue for special logo 'images'
</commit_message>
<xml_diff>
--- a/hw_test3/checkList/check_list.xlsx
+++ b/hw_test3/checkList/check_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>№</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>GW_1</t>
-  </si>
-  <si>
-    <t>GW = Google website</t>
   </si>
   <si>
     <r>
@@ -111,9 +108,6 @@
 3. Google search page with query results correctly open.</t>
   </si>
   <si>
-    <t>Using english lang for browser, so that the name of the button displayed as in this test case description</t>
-  </si>
-  <si>
     <t>GW_4</t>
   </si>
   <si>
@@ -302,13 +296,72 @@
     <t xml:space="preserve">
 1. Img-search page correctly open on Chrome browser
 2. A special window appears for searching by image</t>
+  </si>
+  <si>
+    <t>GW_8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>For all keys:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+GW = Google website
+Using english lang for browser, so that the name of the button displayed as in this test case description</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check that the text is blue for special logo "images"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+1. Open 'https://www.google.com/' with Chrome
+2. Press link "Images" for open img-search page (located in the upper right corner)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Website correctly open on Chrome browser.
+2. Opens img-search page.  Text  "images" for main logo is blue (#4285f4), (rgba(66, 133, 244, 1))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +407,14 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -745,7 +806,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,158 +840,158 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add tet:should correctly displayed panel 'content info' for search results page
</commit_message>
<xml_diff>
--- a/hw_test3/checkList/check_list.xlsx
+++ b/hw_test3/checkList/check_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>№</t>
   </si>
@@ -355,6 +355,33 @@
     <t xml:space="preserve">
 1. Website correctly open on Chrome browser.
 2. Opens img-search page.  Text  "images" for main logo is blue (#4285f4), (rgba(66, 133, 244, 1))</t>
+  </si>
+  <si>
+    <t>GW_9</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check that the panel 'content info' displayed correctly  after opening the search results page:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Open 'https://www.google.com/' with Chrome
+2. Enter a valid query in the search (for example: wikipedia). 
+3. Use key 'Enter'. </t>
+    </r>
+  </si>
+  <si>
+    <t>1. Website correctly open on Chrome browser.
+2. The entered text is displayed correctly in the input field.
+3. Google search page with query results has special panel 'content info' - footer for page</t>
   </si>
 </sst>
 </file>
@@ -464,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -498,6 +525,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +1006,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="8"/>
@@ -994,13 +1024,23 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:7" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add test: should correctly working link 'help' after opening the serch results page:
</commit_message>
<xml_diff>
--- a/hw_test3/checkList/check_list.xlsx
+++ b/hw_test3/checkList/check_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>№</t>
   </si>
@@ -360,6 +360,18 @@
     <t>GW_9</t>
   </si>
   <si>
+    <t>GW_10</t>
+  </si>
+  <si>
+    <t>Content info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Website correctly open on Chrome browser.
+2. The entered text is displayed correctly in the input field.
+3. Google search page with query results has special panel 'content info' - footer for page</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Check that the panel 'content info' displayed correctly  after opening the search results page:
 </t>
@@ -379,9 +391,39 @@
     </r>
   </si>
   <si>
-    <t>1. Website correctly open on Chrome browser.
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check that the panel 'content info' has working link 'help' after opening the serch results page:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Open 'https://www.google.com/' with Chrome
+2. Enter a valid query in the search (for example: wikipedia). 
+3. Use key 'Enter'. 
+4. Click on the link 'help' at the bottom of the screen</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Website correctly open on Chrome browser.
 2. The entered text is displayed correctly in the input field.
-3. Google search page with query results has special panel 'content info' - footer for page</t>
+3. Google search page with query results correctly open.
+4. Google search help correctly opens</t>
   </si>
 </sst>
 </file>
@@ -836,7 +878,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1067,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="8"/>
@@ -1033,23 +1075,33 @@
         <v>18</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: replace sendKeys(val,Key.ENTER) on keyDown and keyUp methods for test check correctly working link 'help'
</commit_message>
<xml_diff>
--- a/hw_test3/checkList/check_list.xlsx
+++ b/hw_test3/checkList/check_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>№</t>
   </si>
@@ -424,6 +424,46 @@
 2. The entered text is displayed correctly in the input field.
 3. Google search page with query results correctly open.
 4. Google search help correctly opens</t>
+  </si>
+  <si>
+    <t>GW_11</t>
+  </si>
+  <si>
+    <t>Google map website</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check that the starting value for zoom = 50km</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Open 'https://www.google.com/maps' with Chrome
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Website correctly open in the Chrome. 
+Start zoom = 50km.</t>
   </si>
 </sst>
 </file>
@@ -542,12 +582,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -570,6 +604,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,7 +918,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,14 +953,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -934,559 +974,569 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>

</xml_diff>

<commit_message>
feat: add test: Google map should have start value for zoom = 50km
</commit_message>
<xml_diff>
--- a/hw_test3/checkList/check_list.xlsx
+++ b/hw_test3/checkList/check_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>№</t>
   </si>
@@ -435,6 +435,11 @@
     <t>Zoom</t>
   </si>
   <si>
+    <t xml:space="preserve">
+1. Website correctly open in the Chrome. 
+Start zoom = 50km.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -445,7 +450,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check that the starting value for zoom = 50km</t>
+      <t>Check that the google map has start value for zoom = 50km</t>
     </r>
     <r>
       <rPr>
@@ -461,9 +466,38 @@
     </r>
   </si>
   <si>
+    <t>GW_12</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check that the increase zoom in is activated by double-clicking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Open 'https://www.google.com/maps' with Chrome
+2. Double-click anywhere on the map.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">
 1. Website correctly open in the Chrome. 
-Start zoom = 50km.</t>
+2. Zoom stay = 20km. The scale is changed visually.</t>
   </si>
 </sst>
 </file>
@@ -573,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -610,6 +644,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,8 +1181,8 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="11"/>
@@ -1156,20 +1193,30 @@
         <v>45</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>